<commit_message>
torque speed characteristics is started to be calculated
</commit_message>
<xml_diff>
--- a/EE 564 - Take Home Exam.xlsx
+++ b/EE 564 - Take Home Exam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elif\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elife\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD1D7A3-26E6-4B86-B6F1-B0DD937FBB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C490EB3F-1444-450D-A30E-74A483EE92A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" tabRatio="776" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.MOTOR DATA" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>Delta</t>
   </si>
@@ -211,18 +211,6 @@
     <t>kws</t>
   </si>
   <si>
-    <t>Bar current (Ib)</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>Do_r (mm)</t>
   </si>
   <si>
@@ -292,20 +280,60 @@
     <t>Magetizing Reactance Calculation</t>
   </si>
   <si>
-    <t>Resultant MMF (FR)</t>
-  </si>
-  <si>
     <t>Core Resistance Calculation</t>
+  </si>
+  <si>
+    <t>Mass (Kg)</t>
+  </si>
+  <si>
+    <t>Mean B (T)</t>
+  </si>
+  <si>
+    <t>Core loss ratio</t>
+  </si>
+  <si>
+    <t>Core loss (Watt)</t>
+  </si>
+  <si>
+    <t>Rc (Ω)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Bar current (Ib, A)</t>
+  </si>
+  <si>
+    <t>Magnetizing Current (A)</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Synchronous speed</t>
+  </si>
+  <si>
+    <t>Slip</t>
+  </si>
+  <si>
+    <t>Synchronous speed (rpm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -551,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,90 +597,80 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1657,27 +1675,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911A2C45-8D9F-484E-AD8C-8733D7AE7273}">
   <dimension ref="B6:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5:T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="S6" s="44" t="s">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
         <v>1</v>
@@ -1689,7 +1707,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1699,7 +1717,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -1709,7 +1727,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -1717,7 +1735,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
         <v>17</v>
@@ -1735,7 +1753,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="7" t="s">
         <v>30</v>
@@ -1744,44 +1762,43 @@
         <v>2</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>37</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="8">
+        <f>120*D10/D11</f>
+        <v>3000</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="4">
-        <v>40</v>
-      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="5" t="s">
         <v>16</v>
@@ -1790,16 +1807,16 @@
         <v>250</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="6">
-        <v>36</v>
+      <c r="F14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="4">
+        <v>40</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="5" t="s">
         <v>6</v>
@@ -1809,38 +1826,38 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="6">
+        <v>36</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6">
+        <v>24.2</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G16" s="6">
         <f>11+11</f>
         <v>22</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="2:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="6">
-        <v>24.2</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="6">
-        <v>2</v>
-      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B17" s="38"/>
-      <c r="C17" s="39" t="s">
+    <row r="17" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="41"/>
+      <c r="C17" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="6">
@@ -1848,34 +1865,33 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="42">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="G17" s="6">
+        <v>2</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41" t="s">
+    <row r="18" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="42"/>
+      <c r="C18" s="27" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="6">
         <v>103</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="8">
-        <f>5*1.1</f>
-        <v>5.5</v>
+      <c r="F18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="6">
+        <v>15</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="7" t="s">
         <v>12</v>
@@ -1884,134 +1900,121 @@
         <v>0.13</v>
       </c>
       <c r="E19" s="2"/>
+      <c r="F19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="8">
+        <f>5*1.1</f>
+        <v>5.5</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B21" s="46" t="s">
+      <c r="E20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4">
         <v>300</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="46"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="43"/>
       <c r="C22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="6">
         <v>170</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B23" s="46"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="43"/>
       <c r="C23" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D23" s="6">
         <v>13</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-    </row>
-    <row r="24" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="46"/>
+    </row>
+    <row r="24" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="43"/>
       <c r="C24" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D24" s="6">
         <v>24</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-    </row>
-    <row r="25" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="46"/>
+    </row>
+    <row r="25" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="43"/>
       <c r="C25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="18">
+        <v>65</v>
+      </c>
+      <c r="D25" s="6">
         <v>3.1</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-    </row>
-    <row r="26" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="46"/>
-      <c r="C26" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="15">
+    </row>
+    <row r="26" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="43"/>
+      <c r="C26" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="8">
         <v>0.87</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B28" s="20" t="s">
+    <row r="27" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>60</v>
+      <c r="C28" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="D28" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B29" s="20"/>
+    <row r="29" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="44"/>
       <c r="C29" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="6">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B30" s="20"/>
+    <row r="30" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="44"/>
       <c r="C30" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D30" s="6">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="20"/>
-      <c r="C31" s="14" t="s">
-        <v>73</v>
+    <row r="31" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="44"/>
+      <c r="C31" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="8">
         <v>24</v>
@@ -2030,26 +2033,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38C05E5-E05C-4416-A759-C6C56C53CC86}">
-  <dimension ref="B3:J20"/>
+  <dimension ref="B3:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="G3" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="C4" s="10" t="s">
         <v>35</v>
@@ -2059,191 +2062,146 @@
       <c r="F4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="33" t="s">
+    <row r="5" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="15">
         <v>54</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="33"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="45"/>
       <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="16">
         <v>70</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="33"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="45"/>
       <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="16">
         <f>954*3</f>
         <v>2862</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="33"/>
-      <c r="C9" s="14" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="45"/>
+      <c r="C9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="17">
         <f>1970*3</f>
         <v>5910</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="21"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="21"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="32" t="s">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="15">
         <v>380</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="32"/>
-      <c r="C16" s="27" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="46"/>
+      <c r="C16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="16">
         <v>17.5</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B17" s="32"/>
-      <c r="C17" s="27" t="s">
+      <c r="E16" s="11"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="46"/>
+      <c r="C17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="16">
         <v>2640</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="32"/>
-      <c r="C18" s="27" t="s">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="46"/>
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="16">
         <v>11300</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="32"/>
-      <c r="C19" s="28" t="s">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="46"/>
+      <c r="C19" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="17">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2257,19 +2215,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D7B3F-248B-4332-8FCD-DF6D0384BDD4}">
-  <dimension ref="C5:Y28"/>
+  <dimension ref="C5:V28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:25" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="10" t="s">
         <v>40</v>
       </c>
@@ -2284,379 +2242,158 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C7" s="56" t="s">
+    <row r="7" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="39">
         <f>'2.TEST DATA'!D19*3/2</f>
         <v>0.153</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-    </row>
-    <row r="8" spans="3:25" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="23">
         <f>'2.TEST DATA'!D18/'1.MOTOR DATA'!D9/('2.TEST DATA'!D16/SQRT(3))^2</f>
         <v>36.897959183673471</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22"/>
-    </row>
-    <row r="9" spans="3:25" ht="18" x14ac:dyDescent="0.35">
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="23">
         <f>4*'2.TEST DATA'!D9/'1.MOTOR DATA'!D9/('2.TEST DATA'!D7/SQRT(3))^2</f>
         <v>4.8244897959183675</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-    </row>
-    <row r="10" spans="3:25" ht="18" x14ac:dyDescent="0.35">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="23">
         <f>'2.TEST DATA'!D8/'1.MOTOR DATA'!D9/('2.TEST DATA'!D7/SQRT(3))^2</f>
         <v>0.58408163265306123</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="22"/>
-    </row>
-    <row r="11" spans="3:25" ht="18" x14ac:dyDescent="0.35">
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="23">
         <f>'2.TEST DATA'!D17-'2.TEST DATA'!D17*0.01-'1.MOTOR DATA'!D9*('2.TEST DATA'!D16/SQRT(3))^2*'3.PARAMETERS (FROM TEST DATA)'!D7</f>
         <v>2566.7437500000001</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22"/>
-    </row>
-    <row r="12" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C12" s="53" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="37">
         <f>'1.MOTOR DATA'!D9*'2.TEST DATA'!D15^2/'3.PARAMETERS (FROM TEST DATA)'!D11</f>
         <v>168.77415207497828</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-    </row>
-    <row r="13" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C13" s="45" t="s">
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-    </row>
-    <row r="14" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C14" s="53" t="s">
+      <c r="D13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C14" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="37">
         <f>(2*D8-SQRT(4*D8^2-4*D9*D8))/2</f>
         <v>2.4967155383023254</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-    </row>
-    <row r="15" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C15" s="53" t="s">
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C15" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="37">
         <f>D14</f>
         <v>2.4967155383023254</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-    </row>
-    <row r="16" spans="3:25" ht="18" x14ac:dyDescent="0.35">
-      <c r="C16" s="53" t="s">
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C16" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="37">
         <f>D8-D14</f>
         <v>34.401243645371146</v>
       </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-    </row>
-    <row r="17" spans="3:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="49" t="s">
+      <c r="P16" s="14"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="32">
         <f>(D10-D7)*((D15+D16)/D16)^2</f>
         <v>0.49592491208751244</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22"/>
-    </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22"/>
-    </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-    </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-    </row>
-    <row r="28" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="H28" s="44" t="s">
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="29" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2671,350 +2408,333 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FE65C8-62DE-4C8C-ACD7-09FA947C1097}">
-  <dimension ref="B5:G36"/>
+  <dimension ref="C5:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F31" sqref="C30:F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="2:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="19"/>
-      <c r="C8" s="59" t="s">
+    <row r="8" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="59"/>
-    </row>
-    <row r="9" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
+      <c r="D8" s="48"/>
+      <c r="F8" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="48"/>
+    </row>
+    <row r="9" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="15">
         <v>1.7199999999999999E-8</v>
       </c>
-      <c r="E9" s="19"/>
       <c r="F9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="15">
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="19"/>
-      <c r="C10" s="51" t="s">
+    <row r="10" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="48">
-        <f>'1.MOTOR DATA'!G14/'1.MOTOR DATA'!D9/'1.MOTOR DATA'!D11</f>
+      <c r="D10" s="16">
+        <f>'1.MOTOR DATA'!G15/'1.MOTOR DATA'!D9/'1.MOTOR DATA'!D11</f>
         <v>6</v>
       </c>
-      <c r="E10" s="19"/>
       <c r="F10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="31">
-        <f>2*G9*D11*'1.MOTOR DATA'!D9/'1.MOTOR DATA'!G13*('1.MOTOR DATA'!G11/3/'1.MOTOR DATA'!G10)</f>
+        <v>88</v>
+      </c>
+      <c r="G10" s="23">
+        <f>2*G9*D11*'1.MOTOR DATA'!D9/'1.MOTOR DATA'!G14*('1.MOTOR DATA'!G11/3/'1.MOTOR DATA'!G10)</f>
         <v>0.6137131578947369</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="19"/>
+    <row r="11" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="48">
-        <f>'1.MOTOR DATA'!G15/2*'1.MOTOR DATA'!G14/'1.MOTOR DATA'!D9</f>
+      <c r="D11" s="16">
+        <f>'1.MOTOR DATA'!G16/2*'1.MOTOR DATA'!G15/'1.MOTOR DATA'!D9</f>
         <v>132</v>
       </c>
-      <c r="E11" s="19"/>
       <c r="F11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="30">
+        <v>85</v>
+      </c>
+      <c r="G11" s="22">
         <f>2/3*G12</f>
         <v>16.133333333333333</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="19"/>
+    <row r="12" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="16">
         <v>15</v>
       </c>
-      <c r="E12" s="19"/>
       <c r="F12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="24">
+        <v>86</v>
+      </c>
+      <c r="G12" s="16">
         <f>'1.MOTOR DATA'!D16</f>
         <v>24.2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="19"/>
+    <row r="13" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="48">
-        <f>'1.MOTOR DATA'!G14/'1.MOTOR DATA'!D11</f>
+      <c r="D13" s="16">
+        <f>'1.MOTOR DATA'!G15/'1.MOTOR DATA'!D11</f>
         <v>18</v>
       </c>
-      <c r="E13" s="19"/>
       <c r="F13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="24">
+        <v>87</v>
+      </c>
+      <c r="G13" s="16">
         <f>('1.MOTOR DATA'!D17-'1.MOTOR DATA'!D18)/2</f>
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="19"/>
+    <row r="14" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="23">
         <f>2*PI()*D12/D13*(('1.MOTOR DATA'!D17-'1.MOTOR DATA'!D18)/2-1)/'1.MOTOR DATA'!D11+2*'1.MOTOR DATA'!D14</f>
         <v>581.15781021773637</v>
       </c>
-      <c r="E14" s="19"/>
       <c r="F14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="24">
+        <v>57</v>
+      </c>
+      <c r="G14" s="16">
         <f>('1.MOTOR DATA'!D17+'1.MOTOR DATA'!D18)/2</f>
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="19"/>
-      <c r="C15" s="49" t="s">
+    <row r="15" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="50">
-        <f>D9*D14*0.001*D11*4/PI()/'1.MOTOR DATA'!G16/'1.MOTOR DATA'!G18/0.000001</f>
+      <c r="D15" s="32">
+        <f>D9*D14*0.001*D11*4/PI()/'1.MOTOR DATA'!G17/'1.MOTOR DATA'!G19/0.000001</f>
         <v>0.1527263210166688</v>
       </c>
-      <c r="E15" s="19"/>
       <c r="F15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="30">
+        <v>58</v>
+      </c>
+      <c r="G15" s="22">
         <f>'1.MOTOR DATA'!D14+2*'4.PARAMETERS ( FROM MOTOR DATA)'!G11+'4.PARAMETERS ( FROM MOTOR DATA)'!G12</f>
         <v>306.46666666666664</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="19"/>
-      <c r="E16" s="19"/>
+    <row r="16" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="30">
+        <v>59</v>
+      </c>
+      <c r="G16" s="22">
         <f>PI()*G14</f>
         <v>424.11500823462205</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C17" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="58"/>
+    <row r="17" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="F17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="24">
+        <v>60</v>
+      </c>
+      <c r="G17" s="16">
         <f>G12*G13</f>
         <v>774.4</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C18" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="17">
-        <f>3/2*4/PI()*SQRT(2)</f>
-        <v>2.7009489484713183</v>
+    <row r="18" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="15">
+        <f>('1.MOTOR DATA'!G10-'1.MOTOR DATA'!G11/3/'1.MOTOR DATA'!G10*SQRT(D15^2+G27^2))/('4.PARAMETERS ( FROM MOTOR DATA)'!D26*0.3)</f>
+        <v>7.3414152311658318</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="30">
+        <v>74</v>
+      </c>
+      <c r="G18" s="22">
         <f>PI()*(8/2)^2</f>
         <v>50.26548245743669</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+    <row r="19" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="51">
+        <f>'1.MOTOR DATA'!G10/'4.PARAMETERS ( FROM MOTOR DATA)'!D18</f>
+        <v>51.76113706071564</v>
+      </c>
       <c r="F19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="29">
+        <v>61</v>
+      </c>
+      <c r="G19" s="21">
         <f>D9*G15/G18*1000</f>
         <v>1.048677225197268E-4</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+    <row r="20" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="29">
-        <f>G19+D9*G14*2*'1.MOTOR DATA'!G13/PI()/'1.MOTOR DATA'!D11^2/'4.PARAMETERS ( FROM MOTOR DATA)'!G17*1000</f>
+        <v>62</v>
+      </c>
+      <c r="G20" s="21">
+        <f>G19+D9*G14*2*'1.MOTOR DATA'!G14/PI()/'1.MOTOR DATA'!D11^2/'4.PARAMETERS ( FROM MOTOR DATA)'!G17*1000</f>
         <v>1.2395645071494276E-4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="F21" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="52">
-        <f>4*'1.MOTOR DATA'!D9*('4.PARAMETERS ( FROM MOTOR DATA)'!D11*'4.PARAMETERS ( FROM MOTOR DATA)'!G9)^2*'4.PARAMETERS ( FROM MOTOR DATA)'!G20/'1.MOTOR DATA'!G13</f>
+    <row r="21" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="F21" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="34">
+        <f>4*'1.MOTOR DATA'!D9*('4.PARAMETERS ( FROM MOTOR DATA)'!D11*'4.PARAMETERS ( FROM MOTOR DATA)'!G9)^2*'4.PARAMETERS ( FROM MOTOR DATA)'!G20/'1.MOTOR DATA'!G14</f>
         <v>0.59094218379853902</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="3:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="58"/>
-      <c r="F24" s="59" t="s">
+    <row r="22" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="59"/>
-    </row>
-    <row r="25" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="F25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="23"/>
-    </row>
-    <row r="26" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="F26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="30">
+      <c r="D22" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="16">
+        <v>270</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="48"/>
+    </row>
+    <row r="24" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="16">
+        <f>D24*D23</f>
+        <v>837</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="22">
         <f>'1.MOTOR DATA'!D24/3/'1.MOTOR DATA'!D23+'1.MOTOR DATA'!D26/'1.MOTOR DATA'!D25</f>
         <v>0.89602977667493799</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="F27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" s="30">
-        <f>0.00003156*'1.MOTOR DATA'!D9*'1.MOTOR DATA'!D10*'4.PARAMETERS ( FROM MOTOR DATA)'!D11^2*('4.PARAMETERS ( FROM MOTOR DATA)'!G26/'1.MOTOR DATA'!G14+'4.PARAMETERS ( FROM MOTOR DATA)'!G26*'1.MOTOR DATA'!D9*'4.PARAMETERS ( FROM MOTOR DATA)'!G9^2/'1.MOTOR DATA'!G13/(2*'1.MOTOR DATA'!G13/'1.MOTOR DATA'!D11))</f>
+    <row r="26" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="32">
+        <f>'1.MOTOR DATA'!G10^2/'4.PARAMETERS ( FROM MOTOR DATA)'!D25</f>
+        <v>172.52090800477896</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="22">
+        <f>0.00003156*'1.MOTOR DATA'!D9*'1.MOTOR DATA'!D10*'4.PARAMETERS ( FROM MOTOR DATA)'!D11^2*('4.PARAMETERS ( FROM MOTOR DATA)'!G25/'1.MOTOR DATA'!G15+'4.PARAMETERS ( FROM MOTOR DATA)'!G25*'1.MOTOR DATA'!D9*'4.PARAMETERS ( FROM MOTOR DATA)'!G9^2/'1.MOTOR DATA'!G14/(2*'1.MOTOR DATA'!G14/'1.MOTOR DATA'!D11))</f>
         <v>2.1794218150175184</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="F28" s="53" t="s">
+    <row r="27" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F27" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="54">
-        <f>G27/2</f>
+      <c r="G27" s="36">
+        <f>G26/2</f>
         <v>1.0897109075087592</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="F29" s="49" t="s">
+    <row r="28" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F28" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="52">
-        <f>G28</f>
+      <c r="G28" s="34">
+        <f>G27</f>
         <v>1.0897109075087592</v>
       </c>
     </row>
-    <row r="30" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="3:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="3:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-    </row>
-    <row r="35" spans="3:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="3:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+    <row r="31" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3022,17 +2742,585 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1344C7-3BF6-498D-905D-A1C1D0C02758}">
-  <dimension ref="C5"/>
+  <dimension ref="A5:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="9.5703125" style="52" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="3:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C5" s="10" t="s">
+    <row r="5" spans="2:3" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="53" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
+        <v>0</v>
+      </c>
+      <c r="C9" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B9)/'1.MOTOR DATA'!$G$12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
+        <v>50</v>
+      </c>
+      <c r="C10" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B10)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.98333333333333328</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
+        <v>100</v>
+      </c>
+      <c r="C11" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B11)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
+        <v>150</v>
+      </c>
+      <c r="C12" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B12)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
+        <v>200</v>
+      </c>
+      <c r="C13" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B13)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
+        <v>250</v>
+      </c>
+      <c r="C14" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B14)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
+        <v>300</v>
+      </c>
+      <c r="C15" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B15)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="52">
+        <v>350</v>
+      </c>
+      <c r="C16" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B16)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.8833333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="52">
+        <v>400</v>
+      </c>
+      <c r="C17" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B17)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="52">
+        <v>450</v>
+      </c>
+      <c r="C18" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B18)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="52">
+        <v>500</v>
+      </c>
+      <c r="C19" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B19)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="52">
+        <v>550</v>
+      </c>
+      <c r="C20" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B20)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.81666666666666665</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="52">
+        <v>600</v>
+      </c>
+      <c r="C21" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B21)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="52">
+        <v>650</v>
+      </c>
+      <c r="C22" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B22)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.78333333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="52">
+        <v>700</v>
+      </c>
+      <c r="C23" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B23)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="52">
+        <v>750</v>
+      </c>
+      <c r="C24" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B24)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="52">
+        <v>800</v>
+      </c>
+      <c r="C25" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B25)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="52">
+        <v>850</v>
+      </c>
+      <c r="C26" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B26)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.71666666666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="52">
+        <v>900</v>
+      </c>
+      <c r="C27" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B27)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="52">
+        <v>950</v>
+      </c>
+      <c r="C28" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B28)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="52">
+        <v>1000</v>
+      </c>
+      <c r="C29" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B29)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="52">
+        <v>1050</v>
+      </c>
+      <c r="C30" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B30)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="52">
+        <v>1100</v>
+      </c>
+      <c r="C31" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B31)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="52">
+        <v>1150</v>
+      </c>
+      <c r="C32" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B32)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="52">
+        <v>1200</v>
+      </c>
+      <c r="C33" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B33)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="52">
+        <v>1250</v>
+      </c>
+      <c r="C34" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B34)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="52">
+        <v>1300</v>
+      </c>
+      <c r="C35" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B35)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="52">
+        <v>1350</v>
+      </c>
+      <c r="C36" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B36)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="52">
+        <v>1400</v>
+      </c>
+      <c r="C37" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B37)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="52">
+        <v>1450</v>
+      </c>
+      <c r="C38" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B38)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.51666666666666672</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="52">
+        <v>1500</v>
+      </c>
+      <c r="C39" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B39)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="52">
+        <v>1550</v>
+      </c>
+      <c r="C40" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B40)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="52">
+        <v>1600</v>
+      </c>
+      <c r="C41" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B41)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="52">
+        <v>1650</v>
+      </c>
+      <c r="C42" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B42)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="52">
+        <v>1700</v>
+      </c>
+      <c r="C43" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B43)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="52">
+        <v>1750</v>
+      </c>
+      <c r="C44" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B44)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="52">
+        <v>1800</v>
+      </c>
+      <c r="C45" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B45)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="52">
+        <v>1850</v>
+      </c>
+      <c r="C46" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B46)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.38333333333333336</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="52">
+        <v>1900</v>
+      </c>
+      <c r="C47" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B47)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="52">
+        <v>1950</v>
+      </c>
+      <c r="C48" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B48)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="52">
+        <v>2000</v>
+      </c>
+      <c r="C49" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B49)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="52">
+        <v>2050</v>
+      </c>
+      <c r="C50" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B50)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.31666666666666665</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="52">
+        <v>2100</v>
+      </c>
+      <c r="C51" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B51)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="52">
+        <v>2150</v>
+      </c>
+      <c r="C52" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B52)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="52">
+        <v>2200</v>
+      </c>
+      <c r="C53" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B53)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="52">
+        <v>2250</v>
+      </c>
+      <c r="C54" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B54)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="52">
+        <v>2300</v>
+      </c>
+      <c r="C55" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B55)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.23333333333333334</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="52">
+        <v>2350</v>
+      </c>
+      <c r="C56" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B56)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.21666666666666667</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="52">
+        <v>2400</v>
+      </c>
+      <c r="C57" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B57)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="52">
+        <v>2450</v>
+      </c>
+      <c r="C58" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B58)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.18333333333333332</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="52">
+        <v>2500</v>
+      </c>
+      <c r="C59" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B59)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="52">
+        <v>2550</v>
+      </c>
+      <c r="C60" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B60)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="52">
+        <v>2600</v>
+      </c>
+      <c r="C61" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B61)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="52">
+        <v>2650</v>
+      </c>
+      <c r="C62" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B62)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.11666666666666667</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="52">
+        <v>2700</v>
+      </c>
+      <c r="C63" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B63)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="52">
+        <v>2750</v>
+      </c>
+      <c r="C64" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B64)/'1.MOTOR DATA'!$G$12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="52">
+        <v>2800</v>
+      </c>
+      <c r="C65" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B65)/'1.MOTOR DATA'!$G$12</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="52">
+        <v>2850</v>
+      </c>
+      <c r="C66" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B66)/'1.MOTOR DATA'!$G$12</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="52">
+        <v>2900</v>
+      </c>
+      <c r="C67" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B67)/'1.MOTOR DATA'!$G$12</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="52">
+        <v>2950</v>
+      </c>
+      <c r="C68" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B68)/'1.MOTOR DATA'!$G$12</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="52">
+        <v>3000</v>
+      </c>
+      <c r="C69" s="52">
+        <f>('1.MOTOR DATA'!$G$12-B69)/'1.MOTOR DATA'!$G$12</f>
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3045,12 +3333,12 @@
   <dimension ref="C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="10" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Hopefullt the last version of the homework
</commit_message>
<xml_diff>
--- a/EE 564 - Take Home Exam.xlsx
+++ b/EE 564 - Take Home Exam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elife\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elif\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7420980-1BE5-4D35-ACF1-8C2B9BD24C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD40E1D-FD56-4F16-8EC5-CC9C5386F944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15390" tabRatio="776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.MOTOR DATA" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
   <si>
     <t>Delta</t>
   </si>
@@ -338,6 +338,15 @@
   <si>
     <t>Since parameters calculated from motor data deviates from the parameters calculated from the test data, the performance of the analytical calculations are less than the test results. But still, the results are pretty close.</t>
   </si>
+  <si>
+    <t>Current Error</t>
+  </si>
+  <si>
+    <t>Torque Error</t>
+  </si>
+  <si>
+    <t>Power Error</t>
+  </si>
 </sst>
 </file>
 
@@ -349,7 +358,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +434,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +749,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,6 +813,15 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Test</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t> Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1582,6 +1627,15 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Test</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR" baseline="0"/>
+              <a:t> Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1690,7 +1744,7 @@
                       </a:pPr>
                       <a:t>[Y DEĞERİ]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="tr-TR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1720,7 +1774,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="tr-TR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
               <c:showLegendKey val="0"/>
@@ -2534,6 +2588,11 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Test Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3340,6 +3399,11 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Motor Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3347,8 +3411,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36181644684254499"/>
-          <c:y val="5.0752607653149984E-2"/>
+          <c:x val="0.23518694354251216"/>
+          <c:y val="5.4972939885538676E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4145,6 +4209,11 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Motor Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4152,8 +4221,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36181644684254499"/>
-          <c:y val="5.0752607653149984E-2"/>
+          <c:x val="0.23962141689844063"/>
+          <c:y val="5.9139057148121024E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4220,78 +4289,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="45"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-5.636403249517212E-2"/>
-                  <c:y val="-0.1706874571713822"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:noAutofit/>
-                  </a:bodyPr>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:fld id="{E82D7530-5DF3-4A6C-8ECC-7F83E3485B94}" type="YVALUE">
-                      <a:rPr lang="en-US" sz="1600"/>
-                      <a:pPr>
-                        <a:defRPr/>
-                      </a:pPr>
-                      <a:t>[Y DEĞERİ]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:noAutofit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="tr-TR"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
+              <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
@@ -4300,11 +4298,30 @@
                       <c:h val="0.11366943657494263"/>
                     </c:manualLayout>
                   </c15:layout>
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-5714-4B9C-9086-1A66E9525885}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="52"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.437962767934525E-2"/>
+                  <c:y val="-4.5693897983875319E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D978-48A9-A8F8-196B09D34497}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4322,7 +4339,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -5097,6 +5114,11 @@
               <a:rPr lang="en-US"/>
               <a:t>vs. Speed</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t> (Motor Data)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -10729,25 +10751,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911A2C45-8D9F-484E-AD8C-8733D7AE7273}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="S2" s="26"/>
     </row>
-    <row r="3" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="2"/>
       <c r="C3" s="10" t="s">
         <v>1</v>
@@ -10761,7 +10783,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -10771,7 +10793,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>18</v>
@@ -10783,7 +10805,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
         <v>17</v>
@@ -10795,7 +10817,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="C7" s="7" t="s">
         <v>28</v>
@@ -10807,7 +10829,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="11"/>
@@ -10815,7 +10837,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
         <v>62</v>
@@ -10827,7 +10849,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -10839,7 +10861,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
         <v>3</v>
@@ -10851,7 +10873,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="2"/>
       <c r="C12" s="7" t="s">
         <v>88</v>
@@ -10864,7 +10886,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="11"/>
@@ -10872,7 +10894,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="3" t="s">
         <v>64</v>
@@ -10884,7 +10906,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="5" t="s">
         <v>63</v>
@@ -10896,7 +10918,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -10909,7 +10931,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
       <c r="C17" s="5" t="s">
         <v>5</v>
@@ -10921,7 +10943,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
       <c r="C18" s="5" t="s">
         <v>44</v>
@@ -10933,7 +10955,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="2"/>
       <c r="C19" s="7" t="s">
         <v>46</v>
@@ -10946,7 +10968,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -10954,7 +10976,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
         <v>68</v>
@@ -10966,7 +10988,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
       <c r="C22" s="5" t="s">
         <v>16</v>
@@ -10978,7 +11000,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="2"/>
       <c r="C23" s="5" t="s">
         <v>6</v>
@@ -10990,7 +11012,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B24" s="54" t="s">
         <v>11</v>
       </c>
@@ -11007,7 +11029,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B25" s="55"/>
       <c r="C25" s="52" t="s">
         <v>14</v>
@@ -11019,7 +11041,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="56"/>
       <c r="C26" s="53" t="s">
         <v>15</v>
@@ -11031,7 +11053,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="2"/>
       <c r="C27" s="7" t="s">
         <v>12</v>
@@ -11043,7 +11065,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -11051,7 +11073,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="54" t="s">
         <v>31</v>
       </c>
@@ -11067,7 +11089,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="55"/>
       <c r="C30" s="52" t="s">
         <v>30</v>
@@ -11078,7 +11100,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B31" s="55"/>
       <c r="C31" s="52" t="s">
         <v>66</v>
@@ -11087,7 +11109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="55"/>
       <c r="C32" s="52" t="s">
         <v>65</v>
@@ -11096,7 +11118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="55"/>
       <c r="C33" s="52" t="s">
         <v>61</v>
@@ -11105,7 +11127,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="56"/>
       <c r="C34" s="53" t="s">
         <v>67</v>
@@ -11114,8 +11136,8 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B36" s="57" t="s">
         <v>32</v>
       </c>
@@ -11126,7 +11148,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B37" s="58"/>
       <c r="C37" s="52" t="s">
         <v>30</v>
@@ -11135,7 +11157,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" s="58"/>
       <c r="C38" s="52" t="s">
         <v>66</v>
@@ -11144,7 +11166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="59"/>
       <c r="C39" s="53" t="s">
         <v>65</v>
@@ -11172,20 +11194,20 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="G3" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="C4" s="10" t="s">
         <v>33</v>
@@ -11195,7 +11217,7 @@
       <c r="F4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -11204,7 +11226,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
         <v>35</v>
       </c>
@@ -11216,7 +11238,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="60"/>
       <c r="C7" s="9" t="s">
         <v>8</v>
@@ -11226,7 +11248,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="60"/>
       <c r="C8" s="9" t="s">
         <v>9</v>
@@ -11237,7 +11259,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="60"/>
       <c r="C9" s="13" t="s">
         <v>19</v>
@@ -11248,39 +11270,39 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B12" s="14"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="11"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="61" t="s">
         <v>10</v>
       </c>
@@ -11295,7 +11317,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="61"/>
       <c r="C16" s="19" t="s">
         <v>8</v>
@@ -11307,7 +11329,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" s="61"/>
       <c r="C17" s="19" t="s">
         <v>9</v>
@@ -11317,7 +11339,7 @@
       </c>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="61"/>
       <c r="C18" s="19" t="s">
         <v>19</v>
@@ -11327,7 +11349,7 @@
       </c>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="61"/>
       <c r="C19" s="20" t="s">
         <v>34</v>
@@ -11354,13 +11376,13 @@
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:22" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:22" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C5" s="10" t="s">
         <v>38</v>
       </c>
@@ -11375,10 +11397,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C7" s="35" t="s">
         <v>37</v>
       </c>
@@ -11387,7 +11409,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="8" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
@@ -11398,7 +11420,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
@@ -11409,7 +11431,7 @@
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
@@ -11420,7 +11442,7 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>97</v>
       </c>
@@ -11431,7 +11453,7 @@
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C12" s="32" t="s">
         <v>27</v>
       </c>
@@ -11449,7 +11471,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C13" s="27" t="s">
         <v>22</v>
       </c>
@@ -11464,7 +11486,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C14" s="32" t="s">
         <v>23</v>
       </c>
@@ -11482,7 +11504,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C15" s="32" t="s">
         <v>25</v>
       </c>
@@ -11500,7 +11522,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="3:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:22" ht="18" x14ac:dyDescent="0.35">
       <c r="C16" s="32" t="s">
         <v>24</v>
       </c>
@@ -11516,7 +11538,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="28" t="s">
         <v>36</v>
       </c>
@@ -11525,7 +11547,7 @@
         <v>0.49592491208751244</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="H28" s="26" t="s">
         <v>48</v>
       </c>
@@ -11547,20 +11569,20 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C5" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C8" s="63" t="s">
         <v>40</v>
       </c>
@@ -11570,7 +11592,7 @@
       </c>
       <c r="G8" s="63"/>
     </row>
-    <row r="9" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>41</v>
       </c>
@@ -11584,7 +11606,7 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="10" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C10" s="30" t="s">
         <v>43</v>
       </c>
@@ -11600,7 +11622,7 @@
         <v>0.6137131578947369</v>
       </c>
     </row>
-    <row r="11" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>42</v>
       </c>
@@ -11616,7 +11638,7 @@
         <v>16.133333333333333</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>44</v>
       </c>
@@ -11631,7 +11653,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
         <v>45</v>
       </c>
@@ -11647,7 +11669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
         <v>49</v>
       </c>
@@ -11663,7 +11685,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="28" t="s">
         <v>50</v>
       </c>
@@ -11679,7 +11701,7 @@
         <v>306.46666666666664</v>
       </c>
     </row>
-    <row r="16" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="F16" s="5" t="s">
         <v>55</v>
       </c>
@@ -11688,7 +11710,7 @@
         <v>424.11500823462205</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C17" s="64" t="s">
         <v>74</v>
       </c>
@@ -11701,7 +11723,7 @@
         <v>774.4</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C18" s="3" t="s">
         <v>85</v>
       </c>
@@ -11717,7 +11739,7 @@
         <v>50.26548245743669</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="28" t="s">
         <v>24</v>
       </c>
@@ -11733,7 +11755,7 @@
         <v>1.048677225197268E-4</v>
       </c>
     </row>
-    <row r="20" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="F20" s="5" t="s">
         <v>58</v>
       </c>
@@ -11742,7 +11764,7 @@
         <v>1.2395645071494276E-4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C21" s="64" t="s">
         <v>75</v>
       </c>
@@ -11755,7 +11777,7 @@
         <v>0.59094218379853902</v>
       </c>
     </row>
-    <row r="22" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C22" s="3" t="s">
         <v>77</v>
       </c>
@@ -11763,7 +11785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C23" s="5" t="s">
         <v>76</v>
       </c>
@@ -11775,7 +11797,7 @@
       </c>
       <c r="G23" s="63"/>
     </row>
-    <row r="24" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C24" s="5" t="s">
         <v>78</v>
       </c>
@@ -11787,7 +11809,7 @@
       </c>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C25" s="5" t="s">
         <v>79</v>
       </c>
@@ -11803,7 +11825,7 @@
         <v>0.89602977667493799</v>
       </c>
     </row>
-    <row r="26" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="28" t="s">
         <v>80</v>
       </c>
@@ -11819,7 +11841,7 @@
         <v>4.7947279930385411</v>
       </c>
     </row>
-    <row r="27" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="F27" s="32" t="s">
         <v>23</v>
       </c>
@@ -11828,7 +11850,7 @@
         <v>2.3973639965192706</v>
       </c>
     </row>
-    <row r="28" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F28" s="28" t="s">
         <v>25</v>
       </c>
@@ -11837,27 +11859,27 @@
         <v>2.3973639965192706</v>
       </c>
     </row>
-    <row r="31" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" ht="18" x14ac:dyDescent="0.35">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" ht="18" x14ac:dyDescent="0.35">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" ht="18" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" ht="18" x14ac:dyDescent="0.35">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" ht="18" x14ac:dyDescent="0.35">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
@@ -11875,28 +11897,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1344C7-3BF6-498D-905D-A1C1D0C02758}">
-  <dimension ref="A4:AA70"/>
+  <dimension ref="A4:AF70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:27" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>94</v>
       </c>
@@ -11912,14 +11936,14 @@
       <c r="Z4" s="66"/>
       <c r="AA4" s="66"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
       <c r="W5" s="66"/>
       <c r="X5" s="66"/>
       <c r="Y5" s="66"/>
       <c r="Z5" s="66"/>
       <c r="AA5" s="66"/>
     </row>
-    <row r="6" spans="2:27" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B6" s="65" t="s">
         <v>95</v>
       </c>
@@ -11940,14 +11964,14 @@
       <c r="Z6" s="66"/>
       <c r="AA6" s="66"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="W7" s="66"/>
       <c r="X7" s="66"/>
       <c r="Y7" s="66"/>
       <c r="Z7" s="66"/>
       <c r="AA7" s="66"/>
     </row>
-    <row r="9" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:32" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="49" t="s">
         <v>93</v>
       </c>
@@ -11979,7 +12003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="41">
         <v>0</v>
       </c>
@@ -12019,7 +12043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" s="44">
         <v>50</v>
       </c>
@@ -12059,7 +12083,7 @@
         <v>0.18418447708931915</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="44">
         <v>100</v>
       </c>
@@ -12099,7 +12123,7 @@
         <v>0.3744701662686783</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" ht="21" x14ac:dyDescent="0.4">
       <c r="B13" s="44">
         <v>150</v>
       </c>
@@ -12138,8 +12162,15 @@
         <f t="shared" si="1"/>
         <v>0.5711598566567142</v>
       </c>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AE13" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF13" s="67">
+        <f>(R10-D10)/D10*100</f>
+        <v>3.779078574346705</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" ht="21" x14ac:dyDescent="0.4">
       <c r="B14" s="44">
         <v>200</v>
       </c>
@@ -12178,8 +12209,15 @@
         <f t="shared" si="1"/>
         <v>0.77457629896794045</v>
       </c>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AE14" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF14" s="68">
+        <f>(S63-E64)/E64*100</f>
+        <v>3.8719122436880693</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="44">
         <v>250</v>
       </c>
@@ -12218,8 +12256,15 @@
         <f t="shared" si="1"/>
         <v>0.9850638380528921</v>
       </c>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AE15" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF15" s="69">
+        <f>(T63-F64)/F64*100</f>
+        <v>1.9483583132493869</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B16" s="44">
         <v>300</v>
       </c>
@@ -12259,7 +12304,7 @@
         <v>1.2029902034611291</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="44">
         <v>350</v>
       </c>
@@ -12299,7 +12344,7 @@
         <v>1.4287484754450568</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="44">
         <v>400</v>
       </c>
@@ -12339,7 +12384,7 @@
         <v>1.662759245923541</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="44">
         <v>450</v>
       </c>
@@ -12379,7 +12424,7 @@
         <v>1.9054729962874952</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="44">
         <v>500</v>
       </c>
@@ -12419,7 +12464,7 @@
         <v>2.1573727165847463</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="44">
         <v>550</v>
       </c>
@@ -12459,7 +12504,7 @@
         <v>2.4189767936000219</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="44">
         <v>600</v>
       </c>
@@ -12499,7 +12544,7 @@
         <v>2.6908421986797384</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="44">
         <v>650</v>
       </c>
@@ -12539,7 +12584,7 @@
         <v>2.973568009871626</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="44">
         <v>700</v>
       </c>
@@ -12579,7 +12624,7 @@
         <v>3.2677993070839872</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B25" s="44">
         <v>750</v>
       </c>
@@ -12619,7 +12664,7 @@
         <v>3.5742314835396303</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B26" s="44">
         <v>800</v>
       </c>
@@ -12659,7 +12704,7 @@
         <v>3.8936150218139058</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" s="44">
         <v>850</v>
       </c>
@@ -12699,7 +12744,7 @@
         <v>4.2267607881930296</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="44">
         <v>900</v>
       </c>
@@ -12739,7 +12784,7 @@
         <v>4.5745459049233528</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" s="44">
         <v>950</v>
       </c>
@@ -12779,7 +12824,7 @@
         <v>4.9379202660498276</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" s="44">
         <v>1000</v>
       </c>
@@ -12819,7 +12864,7 @@
         <v>5.3179137687911036</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="44">
         <v>1050</v>
       </c>
@@ -12859,7 +12904,7 @@
         <v>5.7156443384845739</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="44">
         <v>1100</v>
       </c>
@@ -12899,7 +12944,7 @@
         <v>6.1323268306026693</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B33" s="44">
         <v>1150</v>
       </c>
@@ -12939,7 +12984,7 @@
         <v>6.5692828974880682</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B34" s="44">
         <v>1200</v>
       </c>
@@ -12979,7 +13024,7 @@
         <v>7.027951909210798</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B35" s="44">
         <v>1250</v>
       </c>
@@ -13019,7 +13064,7 @@
         <v>7.5099030157072741</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B36" s="44">
         <v>1300</v>
       </c>
@@ -13059,7 +13104,7 @@
         <v>8.0168484287278137</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B37" s="44">
         <v>1350</v>
       </c>
@@ -13099,7 +13144,7 @@
         <v>8.5506579835488488</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B38" s="44">
         <v>1400</v>
       </c>
@@ -13139,7 +13184,7 @@
         <v>9.1133750066611849</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B39" s="44">
         <v>1450</v>
       </c>
@@ -13179,7 +13224,7 @@
         <v>9.7072334589999194</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B40" s="44">
         <v>1500</v>
       </c>
@@ -13219,7 +13264,7 @@
         <v>10.334676233338108</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B41" s="44">
         <v>1550</v>
       </c>
@@ -13259,7 +13304,7 @@
         <v>10.9983743424</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B42" s="44">
         <v>1600</v>
       </c>
@@ -13299,7 +13344,7 @@
         <v>11.701246516177049</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B43" s="44">
         <v>1650</v>
       </c>
@@ -13339,7 +13384,7 @@
         <v>12.44647839596341</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B44" s="44">
         <v>1700</v>
       </c>
@@ -13379,7 +13424,7 @@
         <v>13.237540013927219</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B45" s="44">
         <v>1750</v>
       </c>
@@ -13419,7 +13464,7 @@
         <v>14.078199498812985</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B46" s="44">
         <v>1800</v>
       </c>
@@ -13459,7 +13504,7 @@
         <v>14.972529828253299</v>
       </c>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B47" s="44">
         <v>1850</v>
       </c>
@@ -13499,7 +13544,7 @@
         <v>15.924903772453346</v>
       </c>
     </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B48" s="44">
         <v>1900</v>
       </c>
@@ -13539,7 +13584,7 @@
         <v>16.939969666145711</v>
       </c>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B49" s="44">
         <v>1950</v>
       </c>
@@ -13579,7 +13624,7 @@
         <v>18.022596888442404</v>
       </c>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B50" s="44">
         <v>2000</v>
       </c>
@@ -13619,7 +13664,7 @@
         <v>19.1777742933597</v>
       </c>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B51" s="44">
         <v>2050</v>
       </c>
@@ -13659,7 +13704,7 @@
         <v>20.410436366449304</v>
       </c>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B52" s="44">
         <v>2100</v>
       </c>
@@ -13699,7 +13744,7 @@
         <v>21.725179155832002</v>
       </c>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B53" s="44">
         <v>2150</v>
       </c>
@@ -13739,7 +13784,7 @@
         <v>23.125808909151665</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B54" s="44">
         <v>2200</v>
       </c>
@@ -13779,7 +13824,7 @@
         <v>24.614637719812123</v>
       </c>
     </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B55" s="44">
         <v>2250</v>
       </c>
@@ -13819,7 +13864,7 @@
         <v>26.191397906732384</v>
       </c>
     </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B56" s="44">
         <v>2300</v>
       </c>
@@ -13859,7 +13904,7 @@
         <v>27.851584354426301</v>
       </c>
     </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B57" s="44">
         <v>2350</v>
       </c>
@@ -13899,7 +13944,7 @@
         <v>29.583944488116146</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B58" s="44">
         <v>2400</v>
       </c>
@@ -13939,7 +13984,7 @@
         <v>31.366712753249409</v>
       </c>
     </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B59" s="44">
         <v>2450</v>
       </c>
@@ -13979,7 +14024,7 @@
         <v>33.162031820260061</v>
       </c>
     </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B60" s="44">
         <v>2500</v>
       </c>
@@ -14019,7 +14064,7 @@
         <v>34.907842700795726</v>
       </c>
     </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B61" s="44">
         <v>2550</v>
       </c>
@@ -14059,7 +14104,7 @@
         <v>36.506452555999694</v>
       </c>
     </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B62" s="44">
         <v>2600</v>
       </c>
@@ -14099,7 +14144,7 @@
         <v>37.809243533856161</v>
       </c>
     </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B63" s="44">
         <v>2650</v>
       </c>
@@ -14139,7 +14184,7 @@
         <v>38.598104802516858</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B64" s="44">
         <v>2700</v>
       </c>
@@ -14179,7 +14224,7 @@
         <v>38.567153692965611</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B65" s="44">
         <v>2750</v>
       </c>
@@ -14219,7 +14264,7 @@
         <v>37.314541593018902</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B66" s="44">
         <v>2800</v>
       </c>
@@ -14259,7 +14304,7 @@
         <v>34.364152101237977</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B67" s="44">
         <v>2850</v>
       </c>
@@ -14299,7 +14344,7 @@
         <v>29.246516782218588</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B68" s="44">
         <v>2900</v>
       </c>
@@ -14339,7 +14384,7 @@
         <v>21.661717855043957</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B69" s="44">
         <v>2950</v>
       </c>
@@ -14379,7 +14424,7 @@
         <v>11.699203854488218</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="50" t="s">
         <v>86</v>
       </c>

</xml_diff>